<commit_message>
Complete work 3 Informatics
</commit_message>
<xml_diff>
--- a/Informatics/Work 3/Работа_3_вар№1_НовопашинАлексейАлександрович.xlsx
+++ b/Informatics/Work 3/Работа_3_вар№1_НовопашинАлексейАлександрович.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Арифметические прогрессии" sheetId="1" r:id="rId1"/>
     <sheet name="Геометрические прогрессии" sheetId="2" r:id="rId2"/>
     <sheet name="Вычисление выражений" sheetId="3" r:id="rId3"/>
     <sheet name="Вычисление функций" sheetId="4" r:id="rId4"/>
+    <sheet name="Приложение 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>d</t>
   </si>
@@ -146,6 +147,114 @@
   </si>
   <si>
     <t>Результат</t>
+  </si>
+  <si>
+    <t>Анализ результатов тестирования</t>
+  </si>
+  <si>
+    <t>Студент</t>
+  </si>
+  <si>
+    <t>Номер задачи</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Номер тестирования</t>
+  </si>
+  <si>
+    <t>Сумма баллов</t>
+  </si>
+  <si>
+    <t>Правильные ответы</t>
+  </si>
+  <si>
+    <t>Полученные баллы</t>
+  </si>
+  <si>
+    <t>Ответы студента</t>
+  </si>
+  <si>
+    <t>Min сумма баллов</t>
+  </si>
+  <si>
+    <t>Оценка</t>
+  </si>
+  <si>
+    <t>Алексеев И.</t>
+  </si>
+  <si>
+    <t>Антонова А.</t>
+  </si>
+  <si>
+    <t>Борисов О.</t>
+  </si>
+  <si>
+    <t>Васильев И.</t>
+  </si>
+  <si>
+    <t>Валова Г.</t>
+  </si>
+  <si>
+    <t>Голубева Р.</t>
+  </si>
+  <si>
+    <t>Денисов П.</t>
+  </si>
+  <si>
+    <t>Количество баллов</t>
+  </si>
+  <si>
+    <t>Петров П.</t>
+  </si>
+  <si>
+    <t>Иванов И.</t>
+  </si>
+  <si>
+    <t>Сидоров С.</t>
+  </si>
+  <si>
+    <t>Анохин М.</t>
+  </si>
+  <si>
+    <t>Неузнавайка Н.</t>
+  </si>
+  <si>
+    <t>Отсчет</t>
+  </si>
+  <si>
+    <t>Критерий</t>
+  </si>
+  <si>
+    <t>Значение</t>
+  </si>
+  <si>
+    <t>Минимальное</t>
+  </si>
+  <si>
+    <t>Максимальное</t>
+  </si>
+  <si>
+    <t>Кол-во студентов, получивших зачет</t>
+  </si>
+  <si>
+    <t>Кол-во студентов, несправившихся с задачами</t>
+  </si>
+  <si>
+    <t>Кол-во студентов, с максимальной суммой баллов</t>
   </si>
 </sst>
 </file>
@@ -190,7 +299,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -341,11 +450,472 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,6 +955,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -392,13 +1014,149 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -423,7 +1181,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -539,11 +1296,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99425792"/>
-        <c:axId val="63740096"/>
+        <c:axId val="98905600"/>
+        <c:axId val="91921152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99425792"/>
+        <c:axId val="98905600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,7 +1337,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63740096"/>
+        <c:crossAx val="91921152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -588,7 +1345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63740096"/>
+        <c:axId val="91921152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,14 +1382,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99425792"/>
+        <c:crossAx val="98905600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -984,21 +1740,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1194,19 +1950,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1379,11 +2135,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1460,7 +2216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -1475,25 +2231,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="61"/>
       <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1903,4 +2659,921 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="6" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="3.5703125" customWidth="1"/>
+    <col min="13" max="13" width="4.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="95" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="95" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="81"/>
+      <c r="N2" s="88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="92"/>
+      <c r="B3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="82"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="89"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="92"/>
+      <c r="B4" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="90" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="92"/>
+      <c r="B5" s="38">
+        <v>3</v>
+      </c>
+      <c r="C5" s="35">
+        <v>2</v>
+      </c>
+      <c r="D5" s="35">
+        <v>2</v>
+      </c>
+      <c r="E5" s="35">
+        <v>4</v>
+      </c>
+      <c r="F5" s="39">
+        <v>3</v>
+      </c>
+      <c r="G5" s="36">
+        <v>1</v>
+      </c>
+      <c r="H5" s="36">
+        <v>2</v>
+      </c>
+      <c r="I5" s="36">
+        <v>2</v>
+      </c>
+      <c r="J5" s="36">
+        <v>3</v>
+      </c>
+      <c r="K5" s="37">
+        <v>4</v>
+      </c>
+      <c r="L5" s="82"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="86" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="87"/>
+      <c r="B6" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="87"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="29">
+        <v>2</v>
+      </c>
+      <c r="C7" s="30">
+        <v>2</v>
+      </c>
+      <c r="D7" s="30">
+        <v>2</v>
+      </c>
+      <c r="E7" s="30">
+        <v>3</v>
+      </c>
+      <c r="F7" s="51">
+        <v>3</v>
+      </c>
+      <c r="G7" s="29">
+        <f>IF(B7=B$5,G$5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" ref="H7:K18" si="0">IF(C7=C$5,H$5,0)</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J7" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="32">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L7" s="90">
+        <f>SUM(G7:K7)</f>
+        <v>8</v>
+      </c>
+      <c r="M7" s="91"/>
+      <c r="N7" s="48" t="str">
+        <f>IF(L7&gt;=$N$4,"зачет","незачет")</f>
+        <v>незачет</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="43">
+        <v>2</v>
+      </c>
+      <c r="G8" s="31">
+        <f t="shared" ref="G8:G18" si="1">IF(B8=B$5,G$5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K8" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="76">
+        <f t="shared" ref="L8:L13" si="2">SUM(G8:K8)</f>
+        <v>5</v>
+      </c>
+      <c r="M8" s="77"/>
+      <c r="N8" s="49" t="str">
+        <f t="shared" ref="N8:N18" si="3">IF(L8&gt;=$N$4,"зачет","незачет")</f>
+        <v>незачет</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="31">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="43">
+        <v>3</v>
+      </c>
+      <c r="G9" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K9" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L9" s="76">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="M9" s="77"/>
+      <c r="N9" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>зачет</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K10" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="76">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="M10" s="77"/>
+      <c r="N10" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>незачет</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="31">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="43">
+        <v>3</v>
+      </c>
+      <c r="G11" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L11" s="76">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M11" s="77"/>
+      <c r="N11" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>незачет</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="41">
+        <v>3</v>
+      </c>
+      <c r="C12" s="42">
+        <v>2</v>
+      </c>
+      <c r="D12" s="42">
+        <v>2</v>
+      </c>
+      <c r="E12" s="42">
+        <v>4</v>
+      </c>
+      <c r="F12" s="52">
+        <v>3</v>
+      </c>
+      <c r="G12" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K12" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L12" s="78">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="M12" s="79"/>
+      <c r="N12" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>зачет</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="31">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13" s="43">
+        <v>3</v>
+      </c>
+      <c r="G13" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K13" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L13" s="69">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="M13" s="70"/>
+      <c r="N13" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>зачет</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="31">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="43">
+        <v>3</v>
+      </c>
+      <c r="G14" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K14" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L14" s="69">
+        <f t="shared" ref="L14:L18" si="4">SUM(G14:K14)</f>
+        <v>12</v>
+      </c>
+      <c r="M14" s="70"/>
+      <c r="N14" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>зачет</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="31"/>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="43">
+        <v>3</v>
+      </c>
+      <c r="G15" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K15" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L15" s="69">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="M15" s="70"/>
+      <c r="N15" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>незачет</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="31">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16" s="43">
+        <v>3</v>
+      </c>
+      <c r="G16" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K16" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L16" s="69">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="M16" s="70"/>
+      <c r="N16" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>незачет</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="31">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+      <c r="F17" s="43">
+        <v>3</v>
+      </c>
+      <c r="G17" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K17" s="33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L17" s="69">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="M17" s="70"/>
+      <c r="N17" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>зачет</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="28">
+        <v>1</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26">
+        <v>4</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="53">
+        <v>3</v>
+      </c>
+      <c r="G18" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="34">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L18" s="71">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M18" s="72"/>
+      <c r="N18" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v>незачет</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="75"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P20" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P21" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q21" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="R21" s="33">
+        <f>MIN(L7:M18)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P22" s="67"/>
+      <c r="Q22" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="R22" s="58">
+        <f>MAX(L7:M18)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q23" s="68"/>
+      <c r="R23" s="33">
+        <f>COUNTIF(N7:N18, "зачет")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q24" s="55">
+        <v>1</v>
+      </c>
+      <c r="R24" s="33">
+        <f>COUNTIF(G7:G18, 0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P25" s="63"/>
+      <c r="Q25" s="55">
+        <v>2</v>
+      </c>
+      <c r="R25" s="33">
+        <f>COUNTIF(H7:H18, 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P26" s="63"/>
+      <c r="Q26" s="55">
+        <v>3</v>
+      </c>
+      <c r="R26" s="33">
+        <f>COUNTIF(I7:I18, 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P27" s="63"/>
+      <c r="Q27" s="55">
+        <v>4</v>
+      </c>
+      <c r="R27" s="33">
+        <f>COUNTIF(J7:J18, 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P28" s="64"/>
+      <c r="Q28" s="55">
+        <v>5</v>
+      </c>
+      <c r="R28" s="33">
+        <f>COUNTIF(K7:K18, 0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="34">
+        <f>COUNTIF(L7:M18, R22)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L2:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="P24:P28"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P21:P22"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N7">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"зачет"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:N18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"зачет"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"зачет"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>